<commit_message>
removed unnecessary old code
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="70">
   <si>
     <t>Flag</t>
   </si>
@@ -71,6 +71,9 @@
     <t>done</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Get Products Negative</t>
   </si>
   <si>
@@ -128,7 +131,7 @@
     <t>Get Category</t>
   </si>
   <si>
-    <t>V1/getCategory</t>
+    <t>v1/getCategory</t>
   </si>
   <si>
     <t>getCategory</t>
@@ -182,6 +185,9 @@
     <t>Get Feed Products</t>
   </si>
   <si>
+    <t>v1/getFeedProducts</t>
+  </si>
+  <si>
     <t>getFeedProducts</t>
   </si>
   <si>
@@ -210,6 +216,9 @@
   </si>
   <si>
     <t>Product Update Notification Negative</t>
+  </si>
+  <si>
+    <t>productBulkUpload</t>
   </si>
   <si>
     <t>getCategorySchemaBulk</t>
@@ -227,10 +236,9 @@
   </numFmts>
   <fonts count="7">
     <font>
-      <b val="true"/>
       <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Abyssinica SIL"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -250,11 +258,12 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Abyssinica SIL"/>
-      <family val="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -315,15 +324,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -340,25 +349,10 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Abyssinica SIL"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -426,23 +420,23 @@
   <dimension ref="1:24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.13617021276596"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.7106382978723"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.0936170212766"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.8936170212766"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.0936170212766"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.3276595744681"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.063829787234"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.60851063829787"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.98723404255319"/>
-    <col collapsed="false" hidden="false" max="936" min="10" style="1" width="9.60851063829787"/>
-    <col collapsed="false" hidden="false" max="1005" min="937" style="2" width="9.60851063829787"/>
-    <col collapsed="false" hidden="false" max="1025" min="1006" style="0" width="9.60851063829787"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.2707423580786"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.5676855895196"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.6724890829694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.2314410480349"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.6986899563319"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.938864628821"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.7205240174672"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.86026200873362"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.1703056768559"/>
+    <col collapsed="false" hidden="false" max="936" min="10" style="1" width="9.86026200873362"/>
+    <col collapsed="false" hidden="false" max="1005" min="937" style="2" width="9.86026200873362"/>
+    <col collapsed="false" hidden="false" max="1025" min="1006" style="0" width="8.62882096069869"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,10 +519,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
@@ -540,13 +534,13 @@
         <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>17</v>
@@ -558,22 +552,22 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>16</v>
@@ -584,28 +578,28 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>17</v>
@@ -616,22 +610,22 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>16</v>
@@ -642,25 +636,25 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>16</v>
@@ -674,22 +668,22 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>16</v>
@@ -700,28 +694,28 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>17</v>
@@ -732,22 +726,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>16</v>
@@ -758,16 +752,16 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>13</v>
@@ -776,10 +770,10 @@
         <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>17</v>
@@ -793,19 +787,19 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>16</v>
@@ -816,28 +810,28 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>17</v>
@@ -848,22 +842,22 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>16</v>
@@ -874,28 +868,28 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>17</v>
@@ -906,22 +900,22 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>16</v>
@@ -932,16 +926,16 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>13</v>
@@ -950,10 +944,10 @@
         <v>13</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>17</v>
@@ -964,10 +958,10 @@
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>12</v>
@@ -979,7 +973,7 @@
         <v>13</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>16</v>
@@ -993,10 +987,10 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>12</v>
@@ -1005,10 +999,10 @@
         <v>13</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>16</v>
@@ -1019,13 +1013,13 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>12</v>
@@ -1037,10 +1031,10 @@
         <v>13</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>17</v>
@@ -1051,22 +1045,22 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>16</v>
@@ -1077,16 +1071,16 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>13</v>
@@ -1095,10 +1089,10 @@
         <v>13</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>17</v>
@@ -1109,22 +1103,22 @@
         <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>16</v>
@@ -1135,16 +1129,16 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>13</v>
@@ -1153,26 +1147,16 @@
         <v>13</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="1:1048576">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A24 L3 S3 Z3 AG3 AN3 AU3 BB3 BI3 BP3 BW3 CD3 CK3 CR3 CY3 DF3 DM3 DT3 EA3 EH3 EO3 EV3 FC3 FJ3 FQ3 FX3 GE3 GL3 GS3 GZ3 HG3 HN3 HU3 IB3 II3 IP3 IW3 JD3 JK3 JR3 JY3 KF3 KM3 KT3 LA3 LH3 LO3 LV3 MC3 MJ3 MQ3 MX3 NE3 NL3 NS3 NZ3 OG3 ON3 OU3 PB3 PI3 PP3 PW3 QD3 QK3 QR3 QY3 RF3 RM3 RT3 SA3 SH3 SO3 SV3 TC3 TJ3 TQ3 TX3 UE3 UL3 US3 UZ3 VG3 VN3 VU3 WB3 WI3 WP3 WW3 XD3 XK3 XR3 XY3 YF3 YM3 YT3 ZA3 ZH3 ZO3 ZV3 AAC3 AAJ3 AAQ3 AAX3 ABE3 ABL3 ABS3 ABZ3 ACG3 ACN3 ACU3 ADB3 ADI3 ADP3 ADW3 AED3 AEK3 AER3 AEY3 AFF3 AFM3 AFT3 AGA3 AGH3 AGO3 AGV3 AHC3 AHJ3 AHQ3 AHX3 AIE3 AIL3 AIS3 AIZ3" type="list">
       <formula1>"Yes,No"</formula1>

</xml_diff>

<commit_message>
before starting extent reporter
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -352,7 +352,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -385,7 +385,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FF99FF99"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -419,8 +419,8 @@
   </sheetPr>
   <dimension ref="1:24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -439,7 +439,7 @@
     <col collapsed="false" hidden="false" max="1025" min="1006" style="0" width="8.62882096069869"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1157,6 +1157,21 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:I30">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A24 L3 S3 Z3 AG3 AN3 AU3 BB3 BI3 BP3 BW3 CD3 CK3 CR3 CY3 DF3 DM3 DT3 EA3 EH3 EO3 EV3 FC3 FJ3 FQ3 FX3 GE3 GL3 GS3 GZ3 HG3 HN3 HU3 IB3 II3 IP3 IW3 JD3 JK3 JR3 JY3 KF3 KM3 KT3 LA3 LH3 LO3 LV3 MC3 MJ3 MQ3 MX3 NE3 NL3 NS3 NZ3 OG3 ON3 OU3 PB3 PI3 PP3 PW3 QD3 QK3 QR3 QY3 RF3 RM3 RT3 SA3 SH3 SO3 SV3 TC3 TJ3 TQ3 TX3 UE3 UL3 US3 UZ3 VG3 VN3 VU3 WB3 WI3 WP3 WW3 XD3 XK3 XR3 XY3 YF3 YM3 YT3 ZA3 ZH3 ZO3 ZV3 AAC3 AAJ3 AAQ3 AAX3 ABE3 ABL3 ABS3 ABZ3 ACG3 ACN3 ACU3 ADB3 ADI3 ADP3 ADW3 AED3 AEK3 AER3 AEY3 AFF3 AFM3 AFT3 AGA3 AGH3 AGO3 AGV3 AHC3 AHJ3 AHQ3 AHX3 AIE3 AIL3 AIS3 AIZ3" type="list">
       <formula1>"Yes,No"</formula1>

</xml_diff>

<commit_message>
started on flask android api testing
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="200" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="200" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="75">
   <si>
     <t>Flag</t>
   </si>
@@ -226,6 +226,21 @@
   </si>
   <si>
     <t>Get Category Schema Negative</t>
+  </si>
+  <si>
+    <t>LoginRequired</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ola@gmail.com</t>
+  </si>
+  <si>
+    <t>RQKmcPib031IxosSb0vTag==</t>
   </si>
 </sst>
 </file>
@@ -235,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <name val="Abyssinica SIL"/>
@@ -273,6 +288,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF3333FF"/>
+      <name val="Abyssinica SIL"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Abyssinica SIL"/>
       <family val="0"/>
       <charset val="1"/>
@@ -320,7 +342,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -338,6 +360,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -430,7 +456,7 @@
   </sheetPr>
   <dimension ref="1:24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1206,8 +1232,8 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1219,11 +1245,14 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.6986899563319"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.938864628821"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.7205240174672"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.86026200873362"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.1703056768559"/>
-    <col collapsed="false" hidden="false" max="936" min="10" style="1" width="9.86026200873362"/>
-    <col collapsed="false" hidden="false" max="1005" min="937" style="2" width="9.86026200873362"/>
-    <col collapsed="false" hidden="false" max="1025" min="1006" style="0" width="8.62882096069869"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.8951965065502"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.7292576419214"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.86026200873362"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.2139737991266"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.1703056768559"/>
+    <col collapsed="false" hidden="false" max="939" min="13" style="1" width="9.86026200873362"/>
+    <col collapsed="false" hidden="false" max="1008" min="940" style="2" width="9.86026200873362"/>
+    <col collapsed="false" hidden="false" max="1025" min="1009" style="0" width="8.62882096069869"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1249,14 +1278,20 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="ALR1" s="0"/>
-      <c r="ALS1" s="0"/>
-      <c r="ALT1" s="0"/>
       <c r="ALU1" s="0"/>
       <c r="ALV1" s="0"/>
       <c r="ALW1" s="0"/>
@@ -1297,12 +1332,21 @@
         <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJA2" s="0"/>
+      <c r="L2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJD2" s="0"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4">
@@ -1315,13 +1359,23 @@
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:I30">
+  <conditionalFormatting sqref="A1:L1,A3:L30,A2:G2,K2:L2">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2 H2" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
added andorid api tests json
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="124">
   <si>
     <t>Flag</t>
   </si>
@@ -228,6 +228,9 @@
     <t>Get Category Schema Negative</t>
   </si>
   <si>
+    <t>RequestHeaders</t>
+  </si>
+  <si>
     <t>LoginRequired</t>
   </si>
   <si>
@@ -237,10 +240,154 @@
     <t>Password</t>
   </si>
   <si>
+    <t>Get Pin code Details</t>
+  </si>
+  <si>
+    <t>1/public/catalog/pincodeDetails</t>
+  </si>
+  <si>
+    <t>android/getPincodeDetails</t>
+  </si>
+  <si>
     <t>ola@gmail.com</t>
   </si>
   <si>
     <t>RQKmcPib031IxosSb0vTag==</t>
+  </si>
+  <si>
+    <t>Get Color Details</t>
+  </si>
+  <si>
+    <t>1/public/catalog/colorDetails</t>
+  </si>
+  <si>
+    <t>android/getColorDetails</t>
+  </si>
+  <si>
+    <t>Trending Search</t>
+  </si>
+  <si>
+    <t>1/public/catalog/trendingSearch</t>
+  </si>
+  <si>
+    <t>android/trendingSearch</t>
+  </si>
+  <si>
+    <t>Get Auto Suggestion</t>
+  </si>
+  <si>
+    <t>1/public/catalog/getAutoSuggestion</t>
+  </si>
+  <si>
+    <t>android/getAutoSuggestion</t>
+  </si>
+  <si>
+    <t>Category Product List</t>
+  </si>
+  <si>
+    <t>1/public/catalog/categoryProductList</t>
+  </si>
+  <si>
+    <t>android/categoryProductList</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>1/public/catalog/search</t>
+  </si>
+  <si>
+    <t>android/search</t>
+  </si>
+  <si>
+    <t>Category Product Count</t>
+  </si>
+  <si>
+    <t>1/public/catalog/categoryProductCount</t>
+  </si>
+  <si>
+    <t>android/categoryProductCount</t>
+  </si>
+  <si>
+    <t>Feed Product List</t>
+  </si>
+  <si>
+    <t>1/public/catalog/feedProductList</t>
+  </si>
+  <si>
+    <t>android/feedProductList</t>
+  </si>
+  <si>
+    <t>Product Details</t>
+  </si>
+  <si>
+    <t>1/public/catalog/productDetail</t>
+  </si>
+  <si>
+    <t>android/productDetail</t>
+  </si>
+  <si>
+    <t>Similar Products</t>
+  </si>
+  <si>
+    <t>1/public/catalog/similarProducts</t>
+  </si>
+  <si>
+    <t>android/similarProducts</t>
+  </si>
+  <si>
+    <t>Check Pin code Availability</t>
+  </si>
+  <si>
+    <t>1/public/checkout/checkPincodeAvailability</t>
+  </si>
+  <si>
+    <t>android/checkPincodeAvailability</t>
+  </si>
+  <si>
+    <t>Is Guest Customer</t>
+  </si>
+  <si>
+    <t>1/public/users/isGuestCustomer</t>
+  </si>
+  <si>
+    <t>android/isGuestCustomer</t>
+  </si>
+  <si>
+    <t>Is Customer Exist</t>
+  </si>
+  <si>
+    <t>1/public/users/isCustomerExist</t>
+  </si>
+  <si>
+    <t>android/isCustomerExist</t>
+  </si>
+  <si>
+    <t>Get Session</t>
+  </si>
+  <si>
+    <t>1/public/users/getSession</t>
+  </si>
+  <si>
+    <t>android/getSession</t>
+  </si>
+  <si>
+    <t>Customer Login</t>
+  </si>
+  <si>
+    <t>1/public/users/customerLogin</t>
+  </si>
+  <si>
+    <t>android/customerLogin</t>
+  </si>
+  <si>
+    <t>Forgot Password</t>
+  </si>
+  <si>
+    <t>1/public/users/forgotPassword</t>
+  </si>
+  <si>
+    <t>android/forgotPassword</t>
   </si>
 </sst>
 </file>
@@ -300,12 +447,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -342,7 +495,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -360,6 +513,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -402,7 +563,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1230,94 +1391,96 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:2"/>
+  <dimension ref="1:17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.2707423580786"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.5676855895196"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.6724890829694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="38.8034934497817"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.2314410480349"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.6986899563319"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.938864628821"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.7205240174672"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.8951965065502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.7292576419214"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.86026200873362"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.2139737991266"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.1703056768559"/>
-    <col collapsed="false" hidden="false" max="939" min="13" style="1" width="9.86026200873362"/>
-    <col collapsed="false" hidden="false" max="1008" min="940" style="2" width="9.86026200873362"/>
-    <col collapsed="false" hidden="false" max="1025" min="1009" style="0" width="8.62882096069869"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.1528384279476"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.8864628820961"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="27.1528384279476"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.8951965065502"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.7292576419214"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.86026200873362"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.2139737991266"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="7.1703056768559"/>
+    <col collapsed="false" hidden="false" max="940" min="14" style="1" width="9.86026200873362"/>
+    <col collapsed="false" hidden="false" max="1009" min="941" style="2" width="9.86026200873362"/>
+    <col collapsed="false" hidden="false" max="1025" min="1010" style="0" width="8.62882096069869"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="ALU1" s="0"/>
-      <c r="ALV1" s="0"/>
-      <c r="ALW1" s="0"/>
-      <c r="ALX1" s="0"/>
-      <c r="ALY1" s="0"/>
-      <c r="ALZ1" s="0"/>
-      <c r="AMA1" s="0"/>
-      <c r="AMB1" s="0"/>
-      <c r="AMC1" s="0"/>
-      <c r="AMD1" s="0"/>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
+      <c r="ALV1" s="6"/>
+      <c r="ALW1" s="6"/>
+      <c r="ALX1" s="6"/>
+      <c r="ALY1" s="6"/>
+      <c r="ALZ1" s="6"/>
+      <c r="AMA1" s="6"/>
+      <c r="AMB1" s="6"/>
+      <c r="AMC1" s="6"/>
+      <c r="AMD1" s="6"/>
+      <c r="AME1" s="6"/>
+      <c r="AMF1" s="6"/>
+      <c r="AMG1" s="6"/>
+      <c r="AMH1" s="6"/>
+      <c r="AMI1" s="6"/>
+      <c r="AMJ1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
@@ -1326,56 +1489,732 @@
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJD2" s="0"/>
+        <v>16</v>
+      </c>
+      <c r="AJE2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJE3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="0"/>
+      <c r="H6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJE17" s="0"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E4">
+  <conditionalFormatting sqref="I2">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
+  <conditionalFormatting sqref="J2">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:L1,A3:L30,A2:G2,K2:L2">
+  <conditionalFormatting sqref="I3">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="J3">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I4">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J4">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7">
+    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9">
+    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10">
+    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11">
+    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12">
+    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
+    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14">
+    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15">
+    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16">
+    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2 H2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A17 I2:I17" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
updated json comparator to ignore given key's value
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="200" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="200" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="133">
   <si>
     <t>Flag</t>
   </si>
@@ -39,6 +39,9 @@
     <t>ExpectedResponse</t>
   </si>
   <si>
+    <t>IgnoreFields</t>
+  </si>
+  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -102,6 +105,9 @@
     <t>expectedResults</t>
   </si>
   <si>
+    <t>message,entity_id,image</t>
+  </si>
+  <si>
     <t>Search Test Negative</t>
   </si>
   <si>
@@ -120,6 +126,9 @@
     <t>expectedProductLite</t>
   </si>
   <si>
+    <t>message</t>
+  </si>
+  <si>
     <t>Product Lite Negative</t>
   </si>
   <si>
@@ -138,6 +147,9 @@
     <t>getCategory</t>
   </si>
   <si>
+    <t>message,data.totalProducts</t>
+  </si>
+  <si>
     <t>Get Category Negative</t>
   </si>
   <si>
@@ -153,6 +165,9 @@
     <t>getVendorProducts</t>
   </si>
   <si>
+    <t>data.totalProducts</t>
+  </si>
+  <si>
     <t>Get Vendor Products Negative</t>
   </si>
   <si>
@@ -165,6 +180,9 @@
     <t>getProducts</t>
   </si>
   <si>
+    <t>d.feedDetails.pageDescription</t>
+  </si>
+  <si>
     <t>noDataFound</t>
   </si>
   <si>
@@ -177,6 +195,9 @@
     <t>getAutosuggestion</t>
   </si>
   <si>
+    <t>message,content.text,content.url_path</t>
+  </si>
+  <si>
     <t>Get Auto suggestion Negative</t>
   </si>
   <si>
@@ -192,6 +213,9 @@
     <t>getFeedProducts</t>
   </si>
   <si>
+    <t>data.feedDetails.pageDescription</t>
+  </si>
+  <si>
     <t>Get Feed Products Negative</t>
   </si>
   <si>
@@ -219,13 +243,16 @@
     <t>Product Update Notification Negative</t>
   </si>
   <si>
+    <t>Product Bulk Upload</t>
+  </si>
+  <si>
     <t>productBulkUpload</t>
   </si>
   <si>
     <t>getCategorySchemaBulk</t>
   </si>
   <si>
-    <t>Get Category Schema Negative</t>
+    <t>Product Bulk Upload Negative</t>
   </si>
   <si>
     <t>RequestHeaders</t>
@@ -495,7 +522,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -514,6 +541,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -617,8 +648,8 @@
   </sheetPr>
   <dimension ref="1:24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -630,14 +661,15 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.6986899563319"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.938864628821"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.7205240174672"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.86026200873362"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.1703056768559"/>
-    <col collapsed="false" hidden="false" max="936" min="10" style="1" width="9.86026200873362"/>
-    <col collapsed="false" hidden="false" max="1005" min="937" style="2" width="9.86026200873362"/>
-    <col collapsed="false" hidden="false" max="1025" min="1006" style="0" width="8.62882096069869"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.0262008733624"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.86026200873362"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.1703056768559"/>
+    <col collapsed="false" hidden="false" max="937" min="11" style="1" width="9.86026200873362"/>
+    <col collapsed="false" hidden="false" max="1006" min="938" style="2" width="9.86026200873362"/>
+    <col collapsed="false" hidden="false" max="1025" min="1007" style="0" width="8.62882096069869"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -665,7 +697,9 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="ALR1" s="0"/>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="ALS1" s="0"/>
       <c r="ALT1" s="0"/>
       <c r="ALU1" s="0"/>
@@ -687,671 +721,700 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="H2" s="0"/>
       <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AJA2" s="0"/>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJB2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="H3" s="0"/>
       <c r="I3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJA3" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJB3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="H5" s="0"/>
       <c r="I5" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="H7" s="0"/>
       <c r="I7" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="H9" s="0"/>
       <c r="I9" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>16</v>
+        <v>48</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="H11" s="0"/>
       <c r="I11" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="H13" s="0"/>
       <c r="I13" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="H15" s="0"/>
       <c r="I15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>16</v>
+        <v>64</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1365,13 +1428,8 @@
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:I30">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A24 L3 S3 Z3 AG3 AN3 AU3 BB3 BI3 BP3 BW3 CD3 CK3 CR3 CY3 DF3 DM3 DT3 EA3 EH3 EO3 EV3 FC3 FJ3 FQ3 FX3 GE3 GL3 GS3 GZ3 HG3 HN3 HU3 IB3 II3 IP3 IW3 JD3 JK3 JR3 JY3 KF3 KM3 KT3 LA3 LH3 LO3 LV3 MC3 MJ3 MQ3 MX3 NE3 NL3 NS3 NZ3 OG3 ON3 OU3 PB3 PI3 PP3 PW3 QD3 QK3 QR3 QY3 RF3 RM3 RT3 SA3 SH3 SO3 SV3 TC3 TJ3 TQ3 TX3 UE3 UL3 US3 UZ3 VG3 VN3 VU3 WB3 WI3 WP3 WW3 XD3 XK3 XR3 XY3 YF3 YM3 YT3 ZA3 ZH3 ZO3 ZV3 AAC3 AAJ3 AAQ3 AAX3 ABE3 ABL3 ABS3 ABZ3 ACG3 ACN3 ACU3 ADB3 ADI3 ADP3 ADW3 AED3 AEK3 AER3 AEY3 AFF3 AFM3 AFT3 AGA3 AGH3 AGO3 AGV3 AHC3 AHJ3 AHQ3 AHX3 AIE3 AIL3 AIS3 AIZ3" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A24 M3 T3 AA3 AH3 AO3 AV3 BC3 BJ3 BQ3 BX3 CE3 CL3 CS3 CZ3 DG3 DN3 DU3 EB3 EI3 EP3 EW3 FD3 FK3 FR3 FY3 GF3 GM3 GT3 HA3 HH3 HO3 HV3 IC3 IJ3 IQ3 IX3 JE3 JL3 JS3 JZ3 KG3 KN3 KU3 LB3 LI3 LP3 LW3 MD3 MK3 MR3 MY3 NF3 NM3 NT3 OA3 OH3 OO3 OV3 PC3 PJ3 PQ3 PX3 QE3 QL3 QS3 QZ3 RG3 RN3 RU3 SB3 SI3 SP3 SW3 TD3 TK3 TR3 TY3 UF3 UM3 UT3 VA3 VH3 VO3 VV3 WC3 WJ3 WQ3 WX3 XE3 XL3 XS3 XZ3 YG3 YN3 YU3 ZB3 ZI3 ZP3 ZW3 AAD3 AAK3 AAR3 AAY3 ABF3 ABM3 ABT3 ACA3 ACH3 ACO3 ACV3 ADC3 ADJ3 ADQ3 ADX3 AEE3 AEL3 AES3 AEZ3 AFG3 AFN3 AFU3 AGB3 AGI3 AGP3 AGW3 AHD3 AHK3 AHR3 AHY3 AIF3 AIM3 AIT3 AJA3" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1393,8 +1451,8 @@
   </sheetPr>
   <dimension ref="1:17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1416,639 +1474,644 @@
     <col collapsed="false" hidden="false" max="1025" min="1010" style="0" width="8.62882096069869"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+    <row r="1" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="I1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="ALV1" s="6"/>
-      <c r="ALW1" s="6"/>
-      <c r="ALX1" s="6"/>
-      <c r="ALY1" s="6"/>
-      <c r="ALZ1" s="6"/>
-      <c r="AMA1" s="6"/>
-      <c r="AMB1" s="6"/>
-      <c r="AMC1" s="6"/>
-      <c r="AMD1" s="6"/>
-      <c r="AME1" s="6"/>
-      <c r="AMF1" s="6"/>
-      <c r="AMG1" s="6"/>
-      <c r="AMH1" s="6"/>
-      <c r="AMI1" s="6"/>
-      <c r="AMJ1" s="6"/>
+      <c r="M1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="ALV1" s="7"/>
+      <c r="ALW1" s="7"/>
+      <c r="ALX1" s="7"/>
+      <c r="ALY1" s="7"/>
+      <c r="ALZ1" s="7"/>
+      <c r="AMA1" s="7"/>
+      <c r="AMB1" s="7"/>
+      <c r="AMC1" s="7"/>
+      <c r="AMD1" s="7"/>
+      <c r="AME1" s="7"/>
+      <c r="AMF1" s="7"/>
+      <c r="AMG1" s="7"/>
+      <c r="AMH1" s="7"/>
+      <c r="AMI1" s="7"/>
+      <c r="AMJ1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="G2" s="0"/>
       <c r="H2" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="M2" s="0"/>
       <c r="AJE2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G3" s="0"/>
       <c r="H3" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G4" s="0"/>
       <c r="H4" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="0"/>
+      <c r="H5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="K5" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>78</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" s="0"/>
       <c r="H6" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJE17" s="0"/>
     </row>

</xml_diff>

<commit_message>
added some cart apis
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="200" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="192" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="149">
   <si>
     <t>Flag</t>
   </si>
@@ -273,10 +273,10 @@
     <t>android/getPincodeDetails</t>
   </si>
   <si>
-    <t>ola@gmail.com</t>
-  </si>
-  <si>
-    <t>RQKmcPib031IxosSb0vTag==</t>
+    <t>cl100@mailinator.com</t>
+  </si>
+  <si>
+    <t>fpF/aIBbNzX/T1RBpbiBTw==</t>
   </si>
   <si>
     <t>Get Color Details</t>
@@ -315,6 +315,9 @@
     <t>android/categoryProductList</t>
   </si>
   <si>
+    <t>pageCount,productCount,totalProducts</t>
+  </si>
+  <si>
     <t>Search</t>
   </si>
   <si>
@@ -333,6 +336,9 @@
     <t>android/categoryProductCount</t>
   </si>
   <si>
+    <t>totalProducts</t>
+  </si>
+  <si>
     <t>Feed Product List</t>
   </si>
   <si>
@@ -378,6 +384,9 @@
     <t>android/isGuestCustomer</t>
   </si>
   <si>
+    <t>token,customerId</t>
+  </si>
+  <si>
     <t>Is Customer Exist</t>
   </si>
   <si>
@@ -396,6 +405,9 @@
     <t>android/getSession</t>
   </si>
   <si>
+    <t>sessionId</t>
+  </si>
+  <si>
     <t>Customer Login</t>
   </si>
   <si>
@@ -435,10 +447,22 @@
     <t>android/addCartSellerNote</t>
   </si>
   <si>
-    <t>3/personal/cart/myCartDetails</t>
-  </si>
-  <si>
-    <t>4/personal/cart/myCartDetails</t>
+    <t>Add to My Cart</t>
+  </si>
+  <si>
+    <t>1/personal/cart/addToMyCart</t>
+  </si>
+  <si>
+    <t>android/addToMyCart</t>
+  </si>
+  <si>
+    <t>Remove from My Cart</t>
+  </si>
+  <si>
+    <t>1/personal/cart/removeFromMyCart</t>
+  </si>
+  <si>
+    <t>android/removeFromMyCart</t>
   </si>
 </sst>
 </file>
@@ -448,7 +472,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <name val="Abyssinica SIL"/>
@@ -486,6 +510,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF3333FF"/>
+      <name val="Abyssinica SIL"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
       <name val="Abyssinica SIL"/>
       <family val="0"/>
       <charset val="1"/>
@@ -546,7 +577,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -580,6 +611,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -673,7 +708,7 @@
   <dimension ref="1:24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="A2:A21 H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1476,7 +1511,7 @@
   <dimension ref="1:21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1556,7 +1591,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>82</v>
@@ -1582,10 +1617,10 @@
       <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -1596,7 +1631,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>87</v>
@@ -1622,10 +1657,10 @@
       <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -1638,7 +1673,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>90</v>
@@ -1664,10 +1699,10 @@
       <c r="I4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -1677,7 +1712,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>93</v>
@@ -1703,10 +1738,10 @@
       <c r="I5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -1714,9 +1749,9 @@
       </c>
       <c r="AJE5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>96</v>
@@ -1736,16 +1771,16 @@
       <c r="G6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>14</v>
+      <c r="H6" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -1753,38 +1788,38 @@
       </c>
       <c r="AJE6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="I7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L7" s="1" t="s">
@@ -1794,36 +1829,36 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>14</v>
+        <v>105</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -1831,38 +1866,38 @@
       </c>
       <c r="AJE8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>14</v>
+        <v>109</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L9" s="1" t="s">
@@ -1872,13 +1907,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>13</v>
@@ -1887,10 +1922,10 @@
         <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>14</v>
@@ -1898,10 +1933,10 @@
       <c r="I10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -1911,13 +1946,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -1926,10 +1961,10 @@
         <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>14</v>
@@ -1937,10 +1972,10 @@
       <c r="I11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L11" s="1" t="s">
@@ -1950,13 +1985,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -1965,10 +2000,10 @@
         <v>14</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>14</v>
@@ -1976,10 +2011,10 @@
       <c r="I12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L12" s="1" t="s">
@@ -1989,36 +2024,36 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L13" s="1" t="s">
@@ -2028,13 +2063,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -2043,10 +2078,10 @@
         <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>14</v>
@@ -2054,10 +2089,10 @@
       <c r="I14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -2067,36 +2102,36 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>14</v>
+        <v>128</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L15" s="1" t="s">
@@ -2106,36 +2141,36 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L16" s="1" t="s">
@@ -2145,25 +2180,25 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>14</v>
@@ -2171,10 +2206,10 @@
       <c r="I17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -2184,25 +2219,25 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>14</v>
@@ -2210,10 +2245,10 @@
       <c r="I18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L18" s="1" t="s">
@@ -2225,22 +2260,22 @@
         <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>14</v>
@@ -2248,10 +2283,10 @@
       <c r="I19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K19" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L19" s="1" t="s">
@@ -2260,25 +2295,25 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>14</v>
@@ -2286,10 +2321,10 @@
       <c r="I20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="K20" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L20" s="1" t="s">
@@ -2298,25 +2333,25 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>14</v>
@@ -2324,10 +2359,10 @@
       <c r="I21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K21" s="9" t="s">
         <v>86</v>
       </c>
       <c r="L21" s="1" t="s">
@@ -2350,158 +2385,83 @@
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3">
+  <conditionalFormatting sqref="I4">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
+  <conditionalFormatting sqref="I5">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
+  <conditionalFormatting sqref="I6">
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
+  <conditionalFormatting sqref="I7">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5">
+  <conditionalFormatting sqref="I8">
     <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
+  <conditionalFormatting sqref="I9">
     <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J6">
+  <conditionalFormatting sqref="I10">
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
+  <conditionalFormatting sqref="I11">
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7">
+  <conditionalFormatting sqref="I12">
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
+  <conditionalFormatting sqref="I13">
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J8">
+  <conditionalFormatting sqref="I14">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
+  <conditionalFormatting sqref="I15">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J9">
+  <conditionalFormatting sqref="I16">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
+  <conditionalFormatting sqref="I17">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J10">
+  <conditionalFormatting sqref="I18:I21">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
+  <conditionalFormatting sqref="J3:J21">
     <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J11">
-    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J12">
-    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J13">
-    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J14">
-    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J15">
-    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J16">
-    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J17">
-    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18:I21">
-    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18:J21">
-    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2511,6 +2471,28 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" display="cl100@mailinator.com"/>
+    <hyperlink ref="J3" r:id="rId2" display="cl100@mailinator.com"/>
+    <hyperlink ref="J4" r:id="rId3" display="cl100@mailinator.com"/>
+    <hyperlink ref="J5" r:id="rId4" display="cl100@mailinator.com"/>
+    <hyperlink ref="J6" r:id="rId5" display="cl100@mailinator.com"/>
+    <hyperlink ref="J7" r:id="rId6" display="cl100@mailinator.com"/>
+    <hyperlink ref="J8" r:id="rId7" display="cl100@mailinator.com"/>
+    <hyperlink ref="J9" r:id="rId8" display="cl100@mailinator.com"/>
+    <hyperlink ref="J10" r:id="rId9" display="cl100@mailinator.com"/>
+    <hyperlink ref="J11" r:id="rId10" display="cl100@mailinator.com"/>
+    <hyperlink ref="J12" r:id="rId11" display="cl100@mailinator.com"/>
+    <hyperlink ref="J13" r:id="rId12" display="cl100@mailinator.com"/>
+    <hyperlink ref="J14" r:id="rId13" display="cl100@mailinator.com"/>
+    <hyperlink ref="J15" r:id="rId14" display="cl100@mailinator.com"/>
+    <hyperlink ref="J16" r:id="rId15" display="cl100@mailinator.com"/>
+    <hyperlink ref="J17" r:id="rId16" display="cl100@mailinator.com"/>
+    <hyperlink ref="J18" r:id="rId17" display="cl100@mailinator.com"/>
+    <hyperlink ref="J19" r:id="rId18" display="cl100@mailinator.com"/>
+    <hyperlink ref="J20" r:id="rId19" display="cl100@mailinator.com"/>
+    <hyperlink ref="J21" r:id="rId20" display="cl100@mailinator.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
added all api positive tests as per swagger doc
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="238">
   <si>
     <t>Flag</t>
   </si>
@@ -279,15 +279,6 @@
     <t>fpF/aIBbNzX/T1RBpbiBTw==</t>
   </si>
   <si>
-    <t>Get Color Details</t>
-  </si>
-  <si>
-    <t>1/public/catalog/colorDetails</t>
-  </si>
-  <si>
-    <t>android/getColorDetails</t>
-  </si>
-  <si>
     <t>Trending Search</t>
   </si>
   <si>
@@ -510,6 +501,24 @@
     <t>android/removeFromMyCart</t>
   </si>
   <si>
+    <t>Attach Address to cart</t>
+  </si>
+  <si>
+    <t>1/personal/cart/attachAddressToCart</t>
+  </si>
+  <si>
+    <t>android/attachAddressToCart</t>
+  </si>
+  <si>
+    <t>Save and Attach Address to cart</t>
+  </si>
+  <si>
+    <t>1/personal/cart/saveAndAttachAddressToCart</t>
+  </si>
+  <si>
+    <t>android/saveAndAttachAddressToCart</t>
+  </si>
+  <si>
     <t>Save New Address</t>
   </si>
   <si>
@@ -567,22 +576,49 @@
     <t>android/updateAddress</t>
   </si>
   <si>
-    <t>Attach Address to cart</t>
-  </si>
-  <si>
-    <t>1/personal/cart/attachAddressToCart</t>
-  </si>
-  <si>
-    <t>android/attachAddressToCart</t>
-  </si>
-  <si>
-    <t>Save and Attach Address to cart</t>
-  </si>
-  <si>
-    <t>1/personal/cart/saveAndAttachAddressToCart</t>
-  </si>
-  <si>
-    <t>android/saveAndAttachAddressToCart</t>
+    <t>Add to wishlist</t>
+  </si>
+  <si>
+    <t>1/personal/users/addToWishlist</t>
+  </si>
+  <si>
+    <t>android/addToWishlist</t>
+  </si>
+  <si>
+    <t>Remove from wishlist</t>
+  </si>
+  <si>
+    <t>1/personal/users/removeFromWishlist</t>
+  </si>
+  <si>
+    <t>android/removeFromWishlist</t>
+  </si>
+  <si>
+    <t>My Wishlist Details</t>
+  </si>
+  <si>
+    <t>1/personal/users/myWishlistDetails</t>
+  </si>
+  <si>
+    <t>android/myWishlistDetails</t>
+  </si>
+  <si>
+    <t>User App Settings</t>
+  </si>
+  <si>
+    <t>1/personal/users/userAppSettings</t>
+  </si>
+  <si>
+    <t>android/userAppSettings</t>
+  </si>
+  <si>
+    <t>Move from wishlist to cart</t>
+  </si>
+  <si>
+    <t>1/personal/cart/moveToCartFromWishlist</t>
+  </si>
+  <si>
+    <t>android/moveToCartFromWishlist</t>
   </si>
   <si>
     <t>Logout</t>
@@ -630,16 +666,70 @@
     <t>android/removeFromMyCartGuest</t>
   </si>
   <si>
-    <t>Attach Address to cart Guest</t>
-  </si>
-  <si>
-    <t>android/attachAddressToCartGuest</t>
-  </si>
-  <si>
     <t>Save and Attach Address to cart Guest</t>
   </si>
   <si>
     <t>android/saveAndAttachAddressToCartGuest</t>
+  </si>
+  <si>
+    <t>User App Settings Guest</t>
+  </si>
+  <si>
+    <t>android/userAppSettingsGuest</t>
+  </si>
+  <si>
+    <t>Get Onboarding Images</t>
+  </si>
+  <si>
+    <t>1/public/users/onboardingImages</t>
+  </si>
+  <si>
+    <t>android/onboardingImages</t>
+  </si>
+  <si>
+    <t>Get Addresses Merchandising Menu</t>
+  </si>
+  <si>
+    <t>1/public/merchandising/menu</t>
+  </si>
+  <si>
+    <t>android/merchandizingMenu</t>
+  </si>
+  <si>
+    <t>Merchandising Dynamic Pages</t>
+  </si>
+  <si>
+    <t>1/public/merchandising/dynamicPage</t>
+  </si>
+  <si>
+    <t>android/merchandizingDynamicPage</t>
+  </si>
+  <si>
+    <t>Config Details</t>
+  </si>
+  <si>
+    <t>1/public/config/configDetails</t>
+  </si>
+  <si>
+    <t>android/configDetails</t>
+  </si>
+  <si>
+    <t>Dynamic URL routes</t>
+  </si>
+  <si>
+    <t>1/public/config/dynamicURLRoutes</t>
+  </si>
+  <si>
+    <t>android/dynamicURLRoutes</t>
+  </si>
+  <si>
+    <t>Marketing Tracking Rules</t>
+  </si>
+  <si>
+    <t>1/public/config/marketingTrackingRules</t>
+  </si>
+  <si>
+    <t>android/marketingTrackingRules</t>
   </si>
 </sst>
 </file>
@@ -881,7 +971,7 @@
   <dimension ref="1:24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="A38:L38 H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1681,10 +1771,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38:L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1835,7 +1925,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>92</v>
@@ -1856,7 +1946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1867,19 +1957,19 @@
         <v>94</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
         <v>95</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>14</v>
+      <c r="H5" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>19</v>
@@ -1899,25 +1989,25 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>19</v>
@@ -1932,7 +2022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1955,7 +2045,7 @@
         <v>102</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>19</v>
@@ -1970,30 +2060,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>19</v>
@@ -2008,7 +2098,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2019,19 +2109,19 @@
         <v>108</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>99</v>
+      <c r="H9" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>19</v>
@@ -2133,19 +2223,19 @@
         <v>117</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>118</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>19</v>
@@ -2165,25 +2255,25 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>122</v>
+        <v>14</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>19</v>
@@ -2209,19 +2299,19 @@
         <v>124</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>125</v>
+        <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>14</v>
+      <c r="H14" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>19</v>
@@ -2241,25 +2331,25 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H15" s="5" t="s">
         <v>129</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>19</v>
@@ -2279,25 +2369,25 @@
         <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>133</v>
+        <v>14</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>19</v>
@@ -2338,7 +2428,7 @@
         <v>14</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>85</v>
@@ -2469,22 +2559,22 @@
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>14</v>
@@ -2507,22 +2597,22 @@
         <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>14</v>
@@ -2753,16 +2843,16 @@
         <v>166</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>167</v>
+        <v>14</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>169</v>
+        <v>86</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>17</v>
@@ -2773,34 +2863,34 @@
         <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="I29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="K29" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>17</v>
@@ -2811,16 +2901,16 @@
         <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>14</v>
@@ -2828,8 +2918,8 @@
       <c r="G30" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="H30" s="5" t="s">
-        <v>133</v>
+      <c r="H30" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>10</v>
@@ -2866,8 +2956,8 @@
       <c r="G31" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>14</v>
+      <c r="H31" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>10</v>
@@ -2987,10 +3077,10 @@
         <v>10</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>85</v>
+        <v>171</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>17</v>
@@ -3025,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>17</v>
@@ -3042,25 +3132,25 @@
         <v>192</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>150</v>
+        <v>193</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J36" s="7" t="s">
         <v>85</v>
@@ -3077,34 +3167,34 @@
         <v>10</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>138</v>
+        <v>196</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>85</v>
+        <v>171</v>
       </c>
       <c r="K37" s="8" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>17</v>
@@ -3115,34 +3205,34 @@
         <v>10</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>141</v>
+        <v>187</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>85</v>
+        <v>171</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>17</v>
@@ -3156,31 +3246,31 @@
         <v>198</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>144</v>
+        <v>199</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>85</v>
+        <v>171</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>17</v>
@@ -3191,34 +3281,34 @@
         <v>10</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>153</v>
+        <v>202</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>85</v>
+        <v>171</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>17</v>
@@ -3229,22 +3319,22 @@
         <v>10</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>14</v>
@@ -3267,22 +3357,22 @@
         <v>10</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>14</v>
@@ -3305,22 +3395,22 @@
         <v>10</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>187</v>
+        <v>138</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>14</v>
@@ -3335,6 +3425,424 @@
         <v>86</v>
       </c>
       <c r="L43" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K48" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K51" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J52" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J53" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K54" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L54" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3419,953 +3927,1068 @@
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
+  <conditionalFormatting sqref="I18">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J18">
+    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V18:V19">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W18:W19">
+    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI18:AI19">
+    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ18:AJ19">
+    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AV18:AV19">
+    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW18:AW19">
+    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BI18:BI19">
+    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BJ18:BJ19">
+    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BV18:BV19">
+    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BW18:BW19">
+    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CI18:CI19">
+    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CJ18:CJ19">
+    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CV18:CV19">
+    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CW18:CW19">
+    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DI18:DI19">
+    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DJ18:DJ19">
+    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DV18:DV19">
+    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DW18:DW19">
+    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="EI18:EI19">
+    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="EJ18:EJ19">
+    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="EV18:EV19">
+    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="EW18:EW19">
+    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="FI18:FI19">
+    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="FJ18:FJ19">
+    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="FV18:FV19">
+    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="FW18:FW19">
+    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="GI18:GI19">
+    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="GJ18:GJ19">
+    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="GV18:GV19">
+    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="GW18:GW19">
+    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="HI18:HI19">
+    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="HJ18:HJ19">
+    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="HV18:HV19">
+    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="HW18:HW19">
+    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="II18:II19">
+    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="IJ18:IJ19">
+    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="IV18:IV19">
+    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="IW18:IW19">
+    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="JI18:JI19">
+    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="JJ18:JJ19">
+    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="JV18:JV19">
+    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="JW18:JW19">
+    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="KI18:KI19">
+    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="KJ18:KJ19">
+    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="KV18:KV19">
+    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="KW18:KW19">
+    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="LI18:LI19">
+    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="LJ18:LJ19">
+    <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="LV18:LV19">
+    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="LW18:LW19">
+    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="MI18:MI19">
+    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="MJ18:MJ19">
+    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="MV18:MV19">
+    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="MW18:MW19">
+    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="NI18:NI19">
+    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="NJ18:NJ19">
+    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="NV18:NV19">
+    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="NW18:NW19">
+    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="OI18:OI19">
+    <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="OJ18:OJ19">
+    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="OV18:OV19">
+    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="OW18:OW19">
+    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="PI18:PI19">
+    <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="PJ18:PJ19">
+    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="PV18:PV19">
+    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="PW18:PW19">
+    <cfRule type="expression" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="QI18:QI19">
+    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="QJ18:QJ19">
+    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="QV18:QV19">
+    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="QW18:QW19">
+    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="RI18:RI19">
+    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="RJ18:RJ19">
+    <cfRule type="expression" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="RV18:RV19">
+    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="RW18:RW19">
+    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="SI18:SI19">
+    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="SJ18:SJ19">
+    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="SV18:SV19">
+    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="SW18:SW19">
+    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="TI18:TI19">
+    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="TJ18:TJ19">
+    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="TV18:TV19">
+    <cfRule type="expression" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="TW18:TW19">
+    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="UI18:UI19">
+    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="UJ18:UJ19">
+    <cfRule type="expression" priority="103" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="UV18:UV19">
+    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="UW18:UW19">
+    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="VI18:VI19">
+    <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="VJ18:VJ19">
+    <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="VV18:VV19">
+    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="VW18:VW19">
+    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="WI18:WI19">
+    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="WJ18:WJ19">
+    <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="WV18:WV19">
+    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="WW18:WW19">
+    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="XI18:XI19">
+    <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="XJ18:XJ19">
+    <cfRule type="expression" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="XV18:XV19">
+    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="XW18:XW19">
+    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="YI18:YI19">
+    <cfRule type="expression" priority="118" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="YJ18:YJ19">
+    <cfRule type="expression" priority="119" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="YV18:YV19">
+    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="YW18:YW19">
+    <cfRule type="expression" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ZI18:ZI19">
+    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ZJ18:ZJ19">
+    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ZV18:ZV19">
+    <cfRule type="expression" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ZW18:ZW19">
+    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AAI18:AAI19">
+    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AAJ18:AAJ19">
+    <cfRule type="expression" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AAV18:AAV19">
+    <cfRule type="expression" priority="128" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AAW18:AAW19">
+    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ABI18:ABI19">
+    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ABJ18:ABJ19">
+    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ABV18:ABV19">
+    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ABW18:ABW19">
+    <cfRule type="expression" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ACI18:ACI19">
+    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ACJ18:ACJ19">
+    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ACV18:ACV19">
+    <cfRule type="expression" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ACW18:ACW19">
+    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ADI18:ADI19">
+    <cfRule type="expression" priority="138" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ADJ18:ADJ19">
+    <cfRule type="expression" priority="139" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ADV18:ADV19">
+    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ADW18:ADW19">
+    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AEI18:AEI19">
+    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AEJ18:AEJ19">
+    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AEV18:AEV19">
+    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AEW18:AEW19">
+    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AFI18:AFI19">
+    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AFJ18:AFJ19">
+    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AFV18:AFV19">
+    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AFW18:AFW19">
+    <cfRule type="expression" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AGI18:AGI19">
+    <cfRule type="expression" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AGJ18:AGJ19">
+    <cfRule type="expression" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AGV18:AGV19">
+    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AGW18:AGW19">
+    <cfRule type="expression" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AHI18:AHI19">
+    <cfRule type="expression" priority="154" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AHJ18:AHJ19">
+    <cfRule type="expression" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AHV18:AHV19">
+    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AHW18:AHW19">
+    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AII18:AII19">
+    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AIJ18:AIJ19">
+    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AIV18:AIV19">
+    <cfRule type="expression" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AIW18:AIW19">
+    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJI18:AJI19">
+    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJJ18:AJJ19">
+    <cfRule type="expression" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJV18:AJV19">
+    <cfRule type="expression" priority="164" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJW18:AJW19">
+    <cfRule type="expression" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AKI18:AKI19">
+    <cfRule type="expression" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AKJ18:AKJ19">
+    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AKV18:AKV19">
+    <cfRule type="expression" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AKW18:AKW19">
+    <cfRule type="expression" priority="169" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ALI18:ALI19">
+    <cfRule type="expression" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ALJ18:ALJ19">
+    <cfRule type="expression" priority="171" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ALV18:ALV19">
+    <cfRule type="expression" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ALW18:ALW19">
+    <cfRule type="expression" priority="173" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AMI18:AMI19">
+    <cfRule type="expression" priority="174" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AMJ18:AMJ19">
+    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24:I25">
+    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J24:J25">
+    <cfRule type="expression" priority="177" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29">
+    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30">
+    <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J30">
+    <cfRule type="expression" priority="181" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
+    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31">
+    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="expression" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J32">
+    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33">
+    <cfRule type="expression" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J33">
+    <cfRule type="expression" priority="187" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40">
+    <cfRule type="expression" priority="189" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19">
-    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V19:V20">
-    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W19:W20">
-    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI19:AI20">
-    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ19:AJ20">
-    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AV19:AV20">
-    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AW19:AW20">
-    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BI19:BI20">
-    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BJ19:BJ20">
-    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BV19:BV20">
-    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BW19:BW20">
-    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CI19:CI20">
-    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CJ19:CJ20">
-    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CV19:CV20">
-    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CW19:CW20">
-    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="DI19:DI20">
-    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="DJ19:DJ20">
-    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="DV19:DV20">
-    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="DW19:DW20">
-    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="EI19:EI20">
-    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="EJ19:EJ20">
-    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="EV19:EV20">
-    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="EW19:EW20">
-    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="FI19:FI20">
-    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="FJ19:FJ20">
-    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="FV19:FV20">
-    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="FW19:FW20">
-    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="GI19:GI20">
-    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="GJ19:GJ20">
-    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="GV19:GV20">
-    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="GW19:GW20">
-    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="HI19:HI20">
-    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="HJ19:HJ20">
-    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="HV19:HV20">
-    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="HW19:HW20">
-    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="II19:II20">
-    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="IJ19:IJ20">
-    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="IV19:IV20">
-    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="IW19:IW20">
-    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="JI19:JI20">
-    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="JJ19:JJ20">
-    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="JV19:JV20">
-    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="JW19:JW20">
-    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="KI19:KI20">
-    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="KJ19:KJ20">
-    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="KV19:KV20">
-    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="KW19:KW20">
-    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="LI19:LI20">
-    <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="LJ19:LJ20">
-    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="LV19:LV20">
-    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="LW19:LW20">
-    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="MI19:MI20">
-    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="MJ19:MJ20">
-    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="MV19:MV20">
-    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="MW19:MW20">
-    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="NI19:NI20">
-    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="NJ19:NJ20">
-    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="NV19:NV20">
-    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="NW19:NW20">
-    <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="OI19:OI20">
-    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="OJ19:OJ20">
-    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="OV19:OV20">
-    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="OW19:OW20">
-    <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="PI19:PI20">
-    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="PJ19:PJ20">
-    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="PV19:PV20">
-    <cfRule type="expression" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="PW19:PW20">
-    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="QI19:QI20">
-    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="QJ19:QJ20">
-    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="QV19:QV20">
-    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="QW19:QW20">
-    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="RI19:RI20">
-    <cfRule type="expression" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="RJ19:RJ20">
-    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="RV19:RV20">
-    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="RW19:RW20">
-    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="SI19:SI20">
-    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="SJ19:SJ20">
-    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="SV19:SV20">
-    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="SW19:SW20">
-    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="TI19:TI20">
-    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="TJ19:TJ20">
-    <cfRule type="expression" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="TV19:TV20">
-    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="TW19:TW20">
-    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="UI19:UI20">
-    <cfRule type="expression" priority="103" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="UJ19:UJ20">
-    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="UV19:UV20">
-    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="UW19:UW20">
-    <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="VI19:VI20">
-    <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="VJ19:VJ20">
-    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="VV19:VV20">
-    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="VW19:VW20">
-    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="WI19:WI20">
-    <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="WJ19:WJ20">
-    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="WV19:WV20">
-    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="WW19:WW20">
-    <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="XI19:XI20">
-    <cfRule type="expression" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="XJ19:XJ20">
-    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="XV19:XV20">
-    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="XW19:XW20">
-    <cfRule type="expression" priority="118" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="YI19:YI20">
-    <cfRule type="expression" priority="119" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="YJ19:YJ20">
-    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="YV19:YV20">
-    <cfRule type="expression" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="YW19:YW20">
-    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ZI19:ZI20">
-    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ZJ19:ZJ20">
-    <cfRule type="expression" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ZV19:ZV20">
-    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ZW19:ZW20">
-    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AAI19:AAI20">
-    <cfRule type="expression" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AAJ19:AAJ20">
-    <cfRule type="expression" priority="128" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AAV19:AAV20">
-    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AAW19:AAW20">
-    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ABI19:ABI20">
-    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ABJ19:ABJ20">
-    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ABV19:ABV20">
-    <cfRule type="expression" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ABW19:ABW20">
-    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ACI19:ACI20">
-    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ACJ19:ACJ20">
-    <cfRule type="expression" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ACV19:ACV20">
-    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ACW19:ACW20">
-    <cfRule type="expression" priority="138" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ADI19:ADI20">
-    <cfRule type="expression" priority="139" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ADJ19:ADJ20">
-    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ADV19:ADV20">
-    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ADW19:ADW20">
-    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AEI19:AEI20">
-    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AEJ19:AEJ20">
-    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AEV19:AEV20">
-    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AEW19:AEW20">
-    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AFI19:AFI20">
-    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AFJ19:AFJ20">
-    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AFV19:AFV20">
-    <cfRule type="expression" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AFW19:AFW20">
-    <cfRule type="expression" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AGI19:AGI20">
-    <cfRule type="expression" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AGJ19:AGJ20">
-    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AGV19:AGV20">
-    <cfRule type="expression" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AGW19:AGW20">
-    <cfRule type="expression" priority="154" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AHI19:AHI20">
-    <cfRule type="expression" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AHJ19:AHJ20">
-    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AHV19:AHV20">
-    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AHW19:AHW20">
-    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AII19:AII20">
-    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AIJ19:AIJ20">
-    <cfRule type="expression" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AIV19:AIV20">
-    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AIW19:AIW20">
-    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJI19:AJI20">
-    <cfRule type="expression" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJJ19:AJJ20">
-    <cfRule type="expression" priority="164" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJV19:AJV20">
-    <cfRule type="expression" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJW19:AJW20">
-    <cfRule type="expression" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AKI19:AKI20">
-    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AKJ19:AKJ20">
-    <cfRule type="expression" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AKV19:AKV20">
-    <cfRule type="expression" priority="169" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AKW19:AKW20">
-    <cfRule type="expression" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ALI19:ALI20">
-    <cfRule type="expression" priority="171" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ALJ19:ALJ20">
-    <cfRule type="expression" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ALV19:ALV20">
-    <cfRule type="expression" priority="173" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ALW19:ALW20">
-    <cfRule type="expression" priority="174" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AMI19:AMI20">
-    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AMJ19:AMJ20">
-    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25:I26">
-    <cfRule type="expression" priority="177" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J25:J26">
-    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="expression" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21">
+    <cfRule type="expression" priority="193" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
+    <cfRule type="expression" priority="194" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J44">
+    <cfRule type="expression" priority="195" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I47">
+    <cfRule type="expression" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J47">
+    <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43">
+    <cfRule type="expression" priority="198" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43">
+    <cfRule type="expression" priority="199" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="expression" priority="200" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J27">
+    <cfRule type="expression" priority="201" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="202" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28">
-    <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="expression" priority="181" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J29">
-    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J30">
-    <cfRule type="expression" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
-    <cfRule type="expression" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="expression" priority="187" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
-    <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="203" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34">
+    <cfRule type="expression" priority="204" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J34">
+    <cfRule type="expression" priority="205" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="expression" priority="206" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J36">
+    <cfRule type="expression" priority="207" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="expression" priority="189" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="208" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35">
-    <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J20">
-    <cfRule type="expression" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="expression" priority="193" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J33">
-    <cfRule type="expression" priority="194" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="expression" priority="195" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J34">
-    <cfRule type="expression" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J22">
-    <cfRule type="expression" priority="198" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="209" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="expression" priority="199" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="210" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="expression" priority="200" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="expression" priority="201" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J42">
-    <cfRule type="expression" priority="202" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
-    <cfRule type="expression" priority="203" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J43">
-    <cfRule type="expression" priority="204" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="211" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
+    <cfRule type="expression" priority="212" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J37">
+    <cfRule type="expression" priority="213" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I48">
+    <cfRule type="expression" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J48">
+    <cfRule type="expression" priority="215" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I49">
+    <cfRule type="expression" priority="216" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J49">
+    <cfRule type="expression" priority="217" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I50">
+    <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J50">
+    <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I51">
+    <cfRule type="expression" priority="220" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J51">
+    <cfRule type="expression" priority="221" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I52">
+    <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J52">
+    <cfRule type="expression" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I53">
+    <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J53">
+    <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I54">
+    <cfRule type="expression" priority="226" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J54">
+    <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="expression" priority="205" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="228" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38">
-    <cfRule type="expression" priority="206" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" priority="229" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A43 I2:I43" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A54 I2:I54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4397,22 +5020,33 @@
     <hyperlink ref="J25" r:id="rId24" display="cl100@mailinator.com"/>
     <hyperlink ref="J26" r:id="rId25" display="cl100@mailinator.com"/>
     <hyperlink ref="J27" r:id="rId26" display="cl100@mailinator.com"/>
-    <hyperlink ref="J28" r:id="rId27" display="cl102@mailinator.com"/>
-    <hyperlink ref="J29" r:id="rId28" display="cl100@mailinator.com"/>
+    <hyperlink ref="J28" r:id="rId27" display="cl100@mailinator.com"/>
+    <hyperlink ref="J29" r:id="rId28" display="cl102@mailinator.com"/>
     <hyperlink ref="J30" r:id="rId29" display="cl100@mailinator.com"/>
     <hyperlink ref="J31" r:id="rId30" display="cl100@mailinator.com"/>
     <hyperlink ref="J32" r:id="rId31" display="cl100@mailinator.com"/>
     <hyperlink ref="J33" r:id="rId32" display="cl100@mailinator.com"/>
-    <hyperlink ref="J34" r:id="rId33" display="cl100@mailinator.com"/>
+    <hyperlink ref="J34" r:id="rId33" display="cl102@mailinator.com"/>
     <hyperlink ref="J35" r:id="rId34" display="cl102@mailinator.com"/>
     <hyperlink ref="J36" r:id="rId35" display="cl100@mailinator.com"/>
-    <hyperlink ref="J37" r:id="rId36" display="cl100@mailinator.com"/>
-    <hyperlink ref="J38" r:id="rId37" display="cl100@mailinator.com"/>
-    <hyperlink ref="J39" r:id="rId38" display="cl100@mailinator.com"/>
-    <hyperlink ref="J40" r:id="rId39" display="cl100@mailinator.com"/>
+    <hyperlink ref="J37" r:id="rId36" display="cl102@mailinator.com"/>
+    <hyperlink ref="J38" r:id="rId37" display="cl102@mailinator.com"/>
+    <hyperlink ref="J39" r:id="rId38" display="cl102@mailinator.com"/>
+    <hyperlink ref="J40" r:id="rId39" display="cl102@mailinator.com"/>
     <hyperlink ref="J41" r:id="rId40" display="cl100@mailinator.com"/>
     <hyperlink ref="J42" r:id="rId41" display="cl100@mailinator.com"/>
     <hyperlink ref="J43" r:id="rId42" display="cl100@mailinator.com"/>
+    <hyperlink ref="J44" r:id="rId43" display="cl100@mailinator.com"/>
+    <hyperlink ref="J45" r:id="rId44" display="cl100@mailinator.com"/>
+    <hyperlink ref="J46" r:id="rId45" display="cl100@mailinator.com"/>
+    <hyperlink ref="J47" r:id="rId46" display="cl100@mailinator.com"/>
+    <hyperlink ref="J48" r:id="rId47" display="cl102@mailinator.com"/>
+    <hyperlink ref="J49" r:id="rId48" display="cl102@mailinator.com"/>
+    <hyperlink ref="J50" r:id="rId49" display="cl102@mailinator.com"/>
+    <hyperlink ref="J51" r:id="rId50" display="cl102@mailinator.com"/>
+    <hyperlink ref="J52" r:id="rId51" display="cl102@mailinator.com"/>
+    <hyperlink ref="J53" r:id="rId52" display="cl102@mailinator.com"/>
+    <hyperlink ref="J54" r:id="rId53" display="cl102@mailinator.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
disabled failed test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="240">
   <si>
     <t>Flag</t>
   </si>
@@ -660,16 +660,22 @@
     <t>android/updateMyCartGuest</t>
   </si>
   <si>
+    <t>Save and Attach Address to cart Guest</t>
+  </si>
+  <si>
+    <t>android/saveAndAttachAddressToCartGuest</t>
+  </si>
+  <si>
+    <t>Apply Coupon Guest</t>
+  </si>
+  <si>
+    <t>Remove Coupon Guest</t>
+  </si>
+  <si>
     <t>Remove from Cart Guest</t>
   </si>
   <si>
     <t>android/removeFromMyCartGuest</t>
-  </si>
-  <si>
-    <t>Save and Attach Address to cart Guest</t>
-  </si>
-  <si>
-    <t>android/saveAndAttachAddressToCartGuest</t>
   </si>
   <si>
     <t>User App Settings Guest</t>
@@ -971,7 +977,7 @@
   <dimension ref="1:24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="A38:L38 H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1771,10 +1777,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38:L38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2594,7 +2600,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>146</v>
@@ -2632,7 +2638,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>149</v>
@@ -2670,7 +2676,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>152</v>
@@ -2708,7 +2714,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>155</v>
@@ -2822,7 +2828,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>164</v>
@@ -2898,7 +2904,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>173</v>
@@ -3050,7 +3056,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>186</v>
@@ -3240,7 +3246,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>198</v>
@@ -3506,13 +3512,13 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>214</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>26</v>
@@ -3544,25 +3550,25 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>217</v>
+        <v>154</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>217</v>
+        <v>154</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>14</v>
@@ -3582,25 +3588,25 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>219</v>
+        <v>157</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>197</v>
+        <v>157</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
@@ -3609,10 +3615,10 @@
         <v>19</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>171</v>
+        <v>85</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>172</v>
+        <v>86</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>17</v>
@@ -3623,22 +3629,22 @@
         <v>10</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>221</v>
+        <v>159</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>14</v>
+        <v>219</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>14</v>
@@ -3647,10 +3653,10 @@
         <v>19</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>171</v>
+        <v>85</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>172</v>
+        <v>86</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>17</v>
@@ -3658,25 +3664,25 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>14</v>
+        <v>221</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
@@ -3696,13 +3702,13 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -3714,7 +3720,7 @@
         <v>14</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>14</v>
@@ -3734,31 +3740,31 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>231</v>
+        <v>14</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="J52" s="7" t="s">
         <v>171</v>
@@ -3772,13 +3778,13 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -3790,7 +3796,7 @@
         <v>14</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>14</v>
@@ -3810,31 +3816,31 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>14</v>
+        <v>233</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J54" s="7" t="s">
         <v>171</v>
@@ -3843,6 +3849,82 @@
         <v>172</v>
       </c>
       <c r="L54" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L56" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4817,12 +4899,12 @@
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
+  <conditionalFormatting sqref="I46">
     <cfRule type="expression" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J47">
+  <conditionalFormatting sqref="J46">
     <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
@@ -4907,72 +4989,72 @@
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I48">
+  <conditionalFormatting sqref="I50">
     <cfRule type="expression" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J48">
+  <conditionalFormatting sqref="J50">
     <cfRule type="expression" priority="215" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I49">
+  <conditionalFormatting sqref="I51">
     <cfRule type="expression" priority="216" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J49">
+  <conditionalFormatting sqref="J51">
     <cfRule type="expression" priority="217" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I50">
+  <conditionalFormatting sqref="I52">
     <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J50">
+  <conditionalFormatting sqref="J52">
     <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I51">
+  <conditionalFormatting sqref="I53">
     <cfRule type="expression" priority="220" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J51">
+  <conditionalFormatting sqref="J53">
     <cfRule type="expression" priority="221" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I52">
+  <conditionalFormatting sqref="I54">
     <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J52">
+  <conditionalFormatting sqref="J54">
     <cfRule type="expression" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I53">
+  <conditionalFormatting sqref="I55">
     <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J53">
+  <conditionalFormatting sqref="J55">
     <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I54">
+  <conditionalFormatting sqref="I56">
     <cfRule type="expression" priority="226" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J54">
+  <conditionalFormatting sqref="J56">
     <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
@@ -4987,8 +5069,18 @@
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I47:I48">
+    <cfRule type="expression" priority="230" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J47:J48">
+    <cfRule type="expression" priority="231" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A54 I2:I54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A56 I2:I56" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5040,13 +5132,15 @@
     <hyperlink ref="J45" r:id="rId44" display="cl100@mailinator.com"/>
     <hyperlink ref="J46" r:id="rId45" display="cl100@mailinator.com"/>
     <hyperlink ref="J47" r:id="rId46" display="cl100@mailinator.com"/>
-    <hyperlink ref="J48" r:id="rId47" display="cl102@mailinator.com"/>
-    <hyperlink ref="J49" r:id="rId48" display="cl102@mailinator.com"/>
+    <hyperlink ref="J48" r:id="rId47" display="cl100@mailinator.com"/>
+    <hyperlink ref="J49" r:id="rId48" display="cl100@mailinator.com"/>
     <hyperlink ref="J50" r:id="rId49" display="cl102@mailinator.com"/>
     <hyperlink ref="J51" r:id="rId50" display="cl102@mailinator.com"/>
     <hyperlink ref="J52" r:id="rId51" display="cl102@mailinator.com"/>
     <hyperlink ref="J53" r:id="rId52" display="cl102@mailinator.com"/>
     <hyperlink ref="J54" r:id="rId53" display="cl102@mailinator.com"/>
+    <hyperlink ref="J55" r:id="rId54" display="cl102@mailinator.com"/>
+    <hyperlink ref="J56" r:id="rId55" display="cl102@mailinator.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
updated as per latest changes
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="135">
   <si>
     <t>Flag</t>
   </si>
@@ -69,6 +69,9 @@
     <t>expectedProducts</t>
   </si>
   <si>
+    <t>seller_ratings</t>
+  </si>
+  <si>
     <t>positive</t>
   </si>
   <si>
@@ -105,7 +108,7 @@
     <t>expectedResults</t>
   </si>
   <si>
-    <t>message,entity_id,image,discount_percentage,url_path,discount_end_date,discount_start_date,name,price</t>
+    <t>message,entity_id,image,discount_percentage,url_path,discount_end_date,discount_start_date,name,price,productCount,totalProducts</t>
   </si>
   <si>
     <t>Search Test Negative</t>
@@ -126,7 +129,7 @@
     <t>expectedProductLite</t>
   </si>
   <si>
-    <t>message</t>
+    <t>message,shipping_cost,is_in_stock</t>
   </si>
   <si>
     <t>Product Lite Negative</t>
@@ -651,8 +654,8 @@
   </sheetPr>
   <dimension ref="1:24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -744,21 +747,23 @@
       <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="0"/>
+      <c r="H2" s="0" t="s">
+        <v>17</v>
+      </c>
       <c r="I2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AJB2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>12</v>
@@ -770,17 +775,17 @@
         <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" s="0"/>
       <c r="I3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AJB3" s="1"/>
     </row>
@@ -789,61 +794,61 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H5" s="0"/>
       <c r="I5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,61 +856,61 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H7" s="0"/>
       <c r="I7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -913,61 +918,61 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H9" s="0"/>
       <c r="I9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,45 +980,45 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
@@ -1022,14 +1027,14 @@
         <v>14</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H11" s="0"/>
       <c r="I11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,58 +1045,58 @@
         <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H13" s="0"/>
       <c r="I13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1099,10 +1104,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -1111,30 +1116,30 @@
         <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
@@ -1143,17 +1148,17 @@
         <v>14</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H15" s="0"/>
       <c r="I15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1161,45 +1166,45 @@
         <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
@@ -1208,14 +1213,14 @@
         <v>14</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H17" s="0"/>
       <c r="I17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1223,10 +1228,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>13</v>
@@ -1238,14 +1243,14 @@
         <v>14</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H18" s="0"/>
       <c r="I18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,10 +1258,10 @@
         <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -1265,30 +1270,30 @@
         <v>14</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -1300,13 +1305,13 @@
         <v>14</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,57 +1319,57 @@
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1372,57 +1377,57 @@
         <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1502,19 +1507,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>8</v>
@@ -1543,10 +1548,10 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -1555,23 +1560,23 @@
         <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G2" s="0"/>
       <c r="H2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M2" s="0"/>
       <c r="AJE2" s="0"/>
@@ -1581,10 +1586,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -1597,22 +1602,22 @@
       </c>
       <c r="G3" s="0"/>
       <c r="H3" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="AJE3" s="0"/>
     </row>
@@ -1621,10 +1626,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -1637,19 +1642,19 @@
       </c>
       <c r="G4" s="0"/>
       <c r="H4" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE4" s="0"/>
     </row>
@@ -1658,10 +1663,10 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -1670,23 +1675,23 @@
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G5" s="0"/>
       <c r="H5" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE5" s="0"/>
     </row>
@@ -1695,35 +1700,35 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="0"/>
       <c r="H6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE6" s="0"/>
     </row>
@@ -1732,34 +1737,34 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE7" s="0"/>
     </row>
@@ -1768,34 +1773,34 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE8" s="0"/>
     </row>
@@ -1804,34 +1809,34 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE9" s="0"/>
     </row>
@@ -1840,10 +1845,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>13</v>
@@ -1852,22 +1857,22 @@
         <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE10" s="0"/>
     </row>
@@ -1876,10 +1881,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -1888,22 +1893,22 @@
         <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE11" s="0"/>
     </row>
@@ -1912,10 +1917,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -1924,22 +1929,22 @@
         <v>14</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE12" s="0"/>
     </row>
@@ -1948,34 +1953,34 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE13" s="0"/>
     </row>
@@ -1984,10 +1989,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -1996,22 +2001,22 @@
         <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE14" s="0"/>
     </row>
@@ -2020,34 +2025,34 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE15" s="0"/>
     </row>
@@ -2056,34 +2061,34 @@
         <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE16" s="0"/>
     </row>
@@ -2092,34 +2097,34 @@
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AJE17" s="0"/>
     </row>

</xml_diff>

<commit_message>
added dynamic filters test
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="200" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="200" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="android" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="dynamic_filters" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="137">
   <si>
     <t>Flag</t>
   </si>
@@ -421,6 +422,12 @@
   </si>
   <si>
     <t>android/forgotPassword</t>
+  </si>
+  <si>
+    <t>Category Dynamic Filters</t>
+  </si>
+  <si>
+    <t>prodCount,filterName</t>
   </si>
 </sst>
 </file>
@@ -654,8 +661,8 @@
   </sheetPr>
   <dimension ref="1:24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2303,4 +2310,108 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.62882096069869"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9825327510917"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9956331877729"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2314410480349"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.117903930131"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.825327510917"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.17903930131"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.6419213973799"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.2139737991266"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.62882096069869"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>